<commit_message>
add indexWeight && share
</commit_message>
<xml_diff>
--- a/vignettes/DataApi.xlsx
+++ b/vignettes/DataApi.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\doc-uibe-data-api\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\qutke\vignettes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1005" yWindow="0" windowWidth="27795" windowHeight="13035" activeTab="1"/>
+    <workbookView xWindow="2010" yWindow="0" windowWidth="27795" windowHeight="13035"/>
   </bookViews>
   <sheets>
     <sheet name="总表" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
   <si>
     <t xml:space="preserve">    分类函数   </t>
   </si>
@@ -36,9 +36,6 @@
     <t xml:space="preserve"> getDailyQuote </t>
   </si>
   <si>
-    <t xml:space="preserve">               </t>
-  </si>
-  <si>
     <t xml:space="preserve"> getIndustry   </t>
   </si>
   <si>
@@ -51,9 +48,6 @@
     <t xml:space="preserve"> qtid                              </t>
   </si>
   <si>
-    <t xml:space="preserve">                                   </t>
-  </si>
-  <si>
     <t xml:space="preserve"> startdate,enddate                 </t>
   </si>
   <si>
@@ -198,6 +192,34 @@
   </si>
   <si>
     <t xml:space="preserve"> 与B相似, 但无需对qtid类似的字段进行优化(如:SecuMarket)                                 </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CompanyCode, date</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加日期</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> getCompanyInfo</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CompanyCode, date都为必填项</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CompanyCode,date</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>getIndexWeight(CSI300指数成份股权重)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>getStockShare(公司股本结构)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -310,7 +332,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -347,13 +369,22 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -637,10 +668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.15"/>
@@ -648,194 +679,223 @@
     <col min="1" max="1" width="22.625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="60.375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="32" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="53.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="1"/>
+    <col min="6" max="6" width="6.75" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="F1" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="4" customFormat="1" ht="33" x14ac:dyDescent="0.15">
+        <v>23</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="4" customFormat="1" ht="33" x14ac:dyDescent="0.15">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="4" customFormat="1" ht="33" x14ac:dyDescent="0.15">
+      <c r="A7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="4" customFormat="1" ht="33" x14ac:dyDescent="0.15">
+      <c r="A8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="11" t="s">
+      <c r="C8" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="4" customFormat="1" ht="33" x14ac:dyDescent="0.15">
-      <c r="A7" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="7" t="s">
+      <c r="D9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="4" customFormat="1" ht="33" x14ac:dyDescent="0.15">
-      <c r="A8" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="7" t="s">
+      <c r="E9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="7" t="s">
+      <c r="E10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>21</v>
-      </c>
       <c r="F10" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="16">
+        <v>42008</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A12" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="16">
+        <v>42008</v>
       </c>
     </row>
   </sheetData>
@@ -856,7 +916,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -868,58 +928,58 @@
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" s="13"/>
+        <v>50</v>
+      </c>
+      <c r="C1" s="12"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" ht="20.25" x14ac:dyDescent="0.15">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
     </row>
     <row r="3" spans="1:6" ht="20.25" x14ac:dyDescent="0.15">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="20.25" x14ac:dyDescent="0.15">
+      <c r="A4" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="20.25" x14ac:dyDescent="0.15">
+      <c r="A5" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="20.25" x14ac:dyDescent="0.15">
-      <c r="A4" s="14" t="s">
+    <row r="6" spans="1:6" ht="20.25" x14ac:dyDescent="0.15">
+      <c r="A6" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B6" s="13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="20.25" x14ac:dyDescent="0.15">
+      <c r="A7" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="13" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="20.25" x14ac:dyDescent="0.15">
-      <c r="A5" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="20.25" x14ac:dyDescent="0.15">
-      <c r="A6" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="20.25" x14ac:dyDescent="0.15">
-      <c r="A7" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>